<commit_message>
updated data and added pollutant data
</commit_message>
<xml_diff>
--- a/Capstone/Data/Korea Population by Region.xlsx
+++ b/Capstone/Data/Korea Population by Region.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="All Data" sheetId="1" r:id="rId1"/>
     <sheet name="Population" sheetId="2" r:id="rId2"/>
+    <sheet name="Projected_Population" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="43">
   <si>
     <t> Period</t>
   </si>
@@ -469,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:MC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="LB1" workbookViewId="0">
+    <sheetView topLeftCell="LB1" workbookViewId="0">
       <selection activeCell="LO11" sqref="LO11"/>
     </sheetView>
   </sheetViews>
@@ -5827,7 +5828,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="R5" sqref="A1:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6118,4 +6119,1535 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U24" sqref="U23:U24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2000</v>
+      </c>
+      <c r="B2">
+        <f>B3-(B12-B7)/5</f>
+        <v>44993251</v>
+      </c>
+      <c r="C2">
+        <f>C3-(C12-C7)/5</f>
+        <v>9970262.9999999963</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:R2" si="0">D3-(D12-D7)/5</f>
+        <v>3802185.9999999995</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>2496609.0000000009</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>2418997.9999999991</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>1287877.9999999998</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>1293557.9999999998</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>979678.99999999977</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>7552869</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>1509462.9999999995</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>1472681.0000000002</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>1801146.9999999998</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>1997324.9999999998</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>2173092.9999999995</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="0"/>
+        <v>2842221</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" si="0"/>
+        <v>2900648.0000000009</v>
+      </c>
+      <c r="R2">
+        <v>494633</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2001</v>
+      </c>
+      <c r="B3">
+        <f>B4-(B12-B7)/5</f>
+        <v>45221821</v>
+      </c>
+      <c r="C3">
+        <f>C4-(C12-C7)/5</f>
+        <v>9955253.799999997</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:R3" si="1">D4-(D12-D7)/5</f>
+        <v>3774325.5999999996</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="1"/>
+        <v>2493402.8000000007</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>2430226.1999999993</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>1300861.7999999998</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>1308487.7999999998</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="1"/>
+        <v>986628.79999999981</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="1"/>
+        <v>7839122</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="1"/>
+        <v>1504972.5999999996</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="1"/>
+        <v>1471458.2000000002</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="1"/>
+        <v>1809981.7999999998</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="1"/>
+        <v>1975993.7999999998</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="1"/>
+        <v>2137765.5999999996</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="1"/>
+        <v>2818763</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="1"/>
+        <v>2916218.8000000007</v>
+      </c>
+      <c r="R3">
+        <v>498358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2002</v>
+      </c>
+      <c r="B4">
+        <f>B5-(B12-B7)/5</f>
+        <v>45450391</v>
+      </c>
+      <c r="C4">
+        <f>C5-(C12-C7)/5</f>
+        <v>9940244.5999999978</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:R4" si="2">D5-(D12-D7)/5</f>
+        <v>3746465.1999999997</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>2490196.6000000006</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>2441454.3999999994</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>1313845.5999999999</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>1323417.5999999999</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>993578.59999999986</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>8125375</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>1500482.1999999997</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>1470235.4000000001</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>1818816.5999999999</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>1954662.5999999999</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="2"/>
+        <v>2102438.1999999997</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="2"/>
+        <v>2795305</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>2931789.6000000006</v>
+      </c>
+      <c r="R4">
+        <v>502083</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2003</v>
+      </c>
+      <c r="B5">
+        <f>B6-(B12-B7)/5</f>
+        <v>45678961</v>
+      </c>
+      <c r="C5">
+        <f>C6-(C12-C7)/5</f>
+        <v>9925235.3999999985</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:R5" si="3">D6-(D12-D7)/5</f>
+        <v>3718604.7999999998</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>2486990.4000000004</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>2452682.5999999996</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>1326829.3999999999</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>1338347.3999999999</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>1000528.3999999999</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>8411628</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>1495991.7999999998</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>1469012.6</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>1827651.4</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>1933331.4</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="3"/>
+        <v>2067110.7999999998</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>2771847</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="3"/>
+        <v>2947360.4000000004</v>
+      </c>
+      <c r="R5">
+        <v>505809</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2004</v>
+      </c>
+      <c r="B6">
+        <f>B7-(B12-B7)/5</f>
+        <v>45907531</v>
+      </c>
+      <c r="C6">
+        <f>C7-(C12-C7)/5</f>
+        <v>9910226.1999999993</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:R6" si="4">D7-(D12-D7)/5</f>
+        <v>3690744.4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="4"/>
+        <v>2483784.2000000002</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="4"/>
+        <v>2463910.7999999998</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>1339813.2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>1353277.2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>1007478.2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>8697881</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>1491501.4</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>1467789.8</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>1836486.2</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>1912000.2</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>2031783.4</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>2748389</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="4"/>
+        <v>2962931.2</v>
+      </c>
+      <c r="R6">
+        <v>509534</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2005</v>
+      </c>
+      <c r="B7" s="1">
+        <v>46136101</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9895217</v>
+      </c>
+      <c r="D7">
+        <v>3662884</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2480578</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2475139</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1352797</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1368207</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1014428</v>
+      </c>
+      <c r="J7" s="1">
+        <v>8984134</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1487011</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1466567</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1845321</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1890669</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1996456</v>
+      </c>
+      <c r="P7" s="1">
+        <v>2724931</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>2978502</v>
+      </c>
+      <c r="R7" s="1">
+        <v>513260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2006</v>
+      </c>
+      <c r="B8">
+        <f>B7+(B12-B7)/5</f>
+        <v>46364671</v>
+      </c>
+      <c r="C8">
+        <f>C7+(C12-C7)/5</f>
+        <v>9880207.8000000007</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:Q8" si="5">D7+(D12-D7)/5</f>
+        <v>3635023.6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="5"/>
+        <v>2477371.7999999998</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="5"/>
+        <v>2486367.2000000002</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="5"/>
+        <v>1365780.8</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="5"/>
+        <v>1383136.8</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>1021377.8</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>9270387</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="5"/>
+        <v>1482520.6</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="5"/>
+        <v>1465344.2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>1854155.8</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="5"/>
+        <v>1869337.8</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>1961128.6</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="5"/>
+        <v>2701473</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="5"/>
+        <v>2994072.8</v>
+      </c>
+      <c r="R8">
+        <f>ROUNDDOWN(R7+(R12-R7)/5,0)</f>
+        <v>516985</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2007</v>
+      </c>
+      <c r="B9">
+        <f>B8+(B12-B7)/5</f>
+        <v>46593241</v>
+      </c>
+      <c r="C9">
+        <f>C8+(C12-C7)/5</f>
+        <v>9865198.6000000015</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:Q9" si="6">D8+(D12-D7)/5</f>
+        <v>3607163.2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="6"/>
+        <v>2474165.5999999996</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="6"/>
+        <v>2497595.4000000004</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="6"/>
+        <v>1378764.6</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="6"/>
+        <v>1398066.6</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="6"/>
+        <v>1028327.6000000001</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="6"/>
+        <v>9556640</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="6"/>
+        <v>1478030.2000000002</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="6"/>
+        <v>1464121.4</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="6"/>
+        <v>1862990.6</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="6"/>
+        <v>1848006.6</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
+        <v>1925801.2000000002</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>2678015</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="6"/>
+        <v>3009643.5999999996</v>
+      </c>
+      <c r="R9">
+        <f>ROUNDDOWN(R8+(R12-R7)/5,0)</f>
+        <v>520710</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2008</v>
+      </c>
+      <c r="B10">
+        <f>B9+(B12-B7)/5</f>
+        <v>46821811</v>
+      </c>
+      <c r="C10">
+        <f>C9+(C12-C7)/5</f>
+        <v>9850189.4000000022</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:Q10" si="7">D9+(D12-D7)/5</f>
+        <v>3579302.8000000003</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="7"/>
+        <v>2470959.3999999994</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="7"/>
+        <v>2508823.6000000006</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="7"/>
+        <v>1391748.4000000001</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="7"/>
+        <v>1412996.4000000001</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="7"/>
+        <v>1035277.4000000001</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="7"/>
+        <v>9842893</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="7"/>
+        <v>1473539.8000000003</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="7"/>
+        <v>1462898.5999999999</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="7"/>
+        <v>1871825.4000000001</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="7"/>
+        <v>1826675.4000000001</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="7"/>
+        <v>1890473.8000000003</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="7"/>
+        <v>2654557</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="7"/>
+        <v>3025214.3999999994</v>
+      </c>
+      <c r="R10">
+        <f>ROUNDDOWN(R9+(R12-R7)/5,0)</f>
+        <v>524435</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2009</v>
+      </c>
+      <c r="B11">
+        <f>B10+(B12-B7)/5</f>
+        <v>47050381</v>
+      </c>
+      <c r="C11">
+        <f>C10+(C12-C7)/5</f>
+        <v>9835180.200000003</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:Q11" si="8">D10+(D12-D7)/5</f>
+        <v>3551442.4000000004</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="8"/>
+        <v>2467753.1999999993</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="8"/>
+        <v>2520051.8000000007</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="8"/>
+        <v>1404732.2000000002</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="8"/>
+        <v>1427926.2000000002</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="8"/>
+        <v>1042227.2000000002</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="8"/>
+        <v>10129146</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="8"/>
+        <v>1469049.4000000004</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="8"/>
+        <v>1461675.7999999998</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="8"/>
+        <v>1880660.2000000002</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="8"/>
+        <v>1805344.2000000002</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="8"/>
+        <v>1855146.4000000004</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="8"/>
+        <v>2631099</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="8"/>
+        <v>3040785.1999999993</v>
+      </c>
+      <c r="R11">
+        <f>ROUNDDOWN(R10+(R12-R7)/5,0)</f>
+        <v>528160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2010</v>
+      </c>
+      <c r="B12" s="1">
+        <v>47278951</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9820171</v>
+      </c>
+      <c r="D12">
+        <v>3523582</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2464547</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2531280</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1417716</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1442856</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1049177</v>
+      </c>
+      <c r="J12" s="1">
+        <v>10415399</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1464559</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1460453</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1889495</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1784013</v>
+      </c>
+      <c r="O12" s="1">
+        <v>1819819</v>
+      </c>
+      <c r="P12" s="1">
+        <v>2607641</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>3056356</v>
+      </c>
+      <c r="R12" s="1">
+        <v>531887</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2011</v>
+      </c>
+      <c r="B13">
+        <f>B12+(B17-B12)/5</f>
+        <v>47539219.399999999</v>
+      </c>
+      <c r="C13">
+        <f>C12+(C17-C12)/5</f>
+        <v>9814997.5999999996</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:Q13" si="9">D12+(D17-D12)/5</f>
+        <v>3501855.6</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="9"/>
+        <v>2460921.2000000002</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="9"/>
+        <v>2557525.7999999998</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="9"/>
+        <v>1429321.8</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="9"/>
+        <v>1454656.6</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="9"/>
+        <v>1055855</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="9"/>
+        <v>10608211</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="9"/>
+        <v>1465949.8</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="9"/>
+        <v>1470793.8</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="9"/>
+        <v>1917196.4</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="9"/>
+        <v>1782654.4</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="9"/>
+        <v>1804155</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="9"/>
+        <v>2606119.2000000002</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="9"/>
+        <v>3077115.6</v>
+      </c>
+      <c r="R13">
+        <f>ROUNDDOWN(R12+(R17-R12)/5,0)</f>
+        <v>531890</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2012</v>
+      </c>
+      <c r="B14">
+        <f>B13+(B17-B12)/5</f>
+        <v>47799487.799999997</v>
+      </c>
+      <c r="C14">
+        <f>C13+(C17-C12)/5</f>
+        <v>9809824.1999999993</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:Q14" si="10">D13+(D17-D12)/5</f>
+        <v>3480129.2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="10"/>
+        <v>2457295.4000000004</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="10"/>
+        <v>2583771.5999999996</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="10"/>
+        <v>1440927.6</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="10"/>
+        <v>1466457.2000000002</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="10"/>
+        <v>1062533</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="10"/>
+        <v>10801023</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="10"/>
+        <v>1467340.6</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="10"/>
+        <v>1481134.6</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="10"/>
+        <v>1944897.7999999998</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="10"/>
+        <v>1781295.7999999998</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="10"/>
+        <v>1788491</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="10"/>
+        <v>2604597.4000000004</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="10"/>
+        <v>3097875.2</v>
+      </c>
+      <c r="R14">
+        <f>ROUNDDOWN(R13+(R17-R12)/5,0)</f>
+        <v>531893</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="B15">
+        <f>B14+(B17-B12)/5</f>
+        <v>48059756.199999996</v>
+      </c>
+      <c r="C15">
+        <f>C14+(C17-C12)/5</f>
+        <v>9804650.7999999989</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:Q15" si="11">D14+(D17-D12)/5</f>
+        <v>3458402.8000000003</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="11"/>
+        <v>2453669.6000000006</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="11"/>
+        <v>2610017.3999999994</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="11"/>
+        <v>1452533.4000000001</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="11"/>
+        <v>1478257.8000000003</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="11"/>
+        <v>1069211</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="11"/>
+        <v>10993835</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="11"/>
+        <v>1468731.4000000001</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="11"/>
+        <v>1491475.4000000001</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="11"/>
+        <v>1972599.1999999997</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="11"/>
+        <v>1779937.1999999997</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="11"/>
+        <v>1772827</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="11"/>
+        <v>2603075.6000000006</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="11"/>
+        <v>3118634.8000000003</v>
+      </c>
+      <c r="R15">
+        <f>ROUNDDOWN(R14+(R17-R12)/5,0)</f>
+        <v>531896</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2014</v>
+      </c>
+      <c r="B16">
+        <f>B15+(B17-B12)/5</f>
+        <v>48320024.599999994</v>
+      </c>
+      <c r="C16">
+        <f>C15+(C17-C12)/5</f>
+        <v>9799477.3999999985</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:Q16" si="12">D15+(D17-D12)/5</f>
+        <v>3436676.4000000004</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="12"/>
+        <v>2450043.8000000007</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="12"/>
+        <v>2636263.1999999993</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="12"/>
+        <v>1464139.2000000002</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="12"/>
+        <v>1490058.4000000004</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="12"/>
+        <v>1075889</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="12"/>
+        <v>11186647</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="12"/>
+        <v>1470122.2000000002</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="12"/>
+        <v>1501816.2000000002</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="12"/>
+        <v>2000300.5999999996</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="12"/>
+        <v>1778578.5999999996</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="12"/>
+        <v>1757163</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="12"/>
+        <v>2601553.8000000007</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="12"/>
+        <v>3139394.4000000004</v>
+      </c>
+      <c r="R16">
+        <f>ROUNDDOWN(R15+(R17-R12)/5,0)</f>
+        <v>531899</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2015</v>
+      </c>
+      <c r="B17" s="1">
+        <v>48580293</v>
+      </c>
+      <c r="C17" s="1">
+        <v>9794304</v>
+      </c>
+      <c r="D17">
+        <v>3414950</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2446418</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2662509</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1475745</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1501859</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1082567</v>
+      </c>
+      <c r="J17" s="1">
+        <v>11379459</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1471513</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1512157</v>
+      </c>
+      <c r="M17" s="1">
+        <v>2028002</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1777220</v>
+      </c>
+      <c r="O17" s="1">
+        <v>1741499</v>
+      </c>
+      <c r="P17" s="1">
+        <v>2600032</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>3160154</v>
+      </c>
+      <c r="R17" s="1">
+        <v>531905</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2016</v>
+      </c>
+      <c r="B18">
+        <f>B17+(B22-B17)/5</f>
+        <v>49211848.600000001</v>
+      </c>
+      <c r="C18">
+        <f>C17+(C22-C17)/5</f>
+        <v>9729868.5999999996</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:Q18" si="13">D17+(D22-D17)/5</f>
+        <v>3396827</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="13"/>
+        <v>2434716.6</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="13"/>
+        <v>2721416</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="13"/>
+        <v>1475648.4</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="13"/>
+        <v>1497435.2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="13"/>
+        <v>1090204.2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="13"/>
+        <v>11834073</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="13"/>
+        <v>1481588.4</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="13"/>
+        <v>1534678.4</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="13"/>
+        <v>2057593.6</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="13"/>
+        <v>1779186.6</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="13"/>
+        <v>1748824</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="13"/>
+        <v>2607088.4</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="13"/>
+        <v>3189309.4</v>
+      </c>
+      <c r="R18">
+        <f>ROUNDDOWN(R17+(R22-R17)/5,0)</f>
+        <v>560145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2017</v>
+      </c>
+      <c r="B19">
+        <f>B18+(B22-B17)/5</f>
+        <v>49843404.200000003</v>
+      </c>
+      <c r="C19">
+        <f>C18+(C22-C17)/5</f>
+        <v>9665433.1999999993</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:Q19" si="14">D18+(D22-D17)/5</f>
+        <v>3378704</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="14"/>
+        <v>2423015.2000000002</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="14"/>
+        <v>2780323</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="14"/>
+        <v>1475551.7999999998</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="14"/>
+        <v>1493011.4</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="14"/>
+        <v>1097841.3999999999</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="14"/>
+        <v>12288687</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="14"/>
+        <v>1491663.7999999998</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="14"/>
+        <v>1557199.7999999998</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="14"/>
+        <v>2087185.2000000002</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="14"/>
+        <v>1781153.2000000002</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="14"/>
+        <v>1756149</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="14"/>
+        <v>2614144.7999999998</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="14"/>
+        <v>3218464.8</v>
+      </c>
+      <c r="R19">
+        <f>ROUNDDOWN(R18+(R22-R17)/5,0)</f>
+        <v>588385</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2018</v>
+      </c>
+      <c r="B20">
+        <f>B19+(B22-B17)/5</f>
+        <v>50474959.800000004</v>
+      </c>
+      <c r="C20">
+        <f>C19+(C22-C17)/5</f>
+        <v>9600997.7999999989</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:Q20" si="15">D19+(D22-D17)/5</f>
+        <v>3360581</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="15"/>
+        <v>2411313.8000000003</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="15"/>
+        <v>2839230</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="15"/>
+        <v>1475455.1999999997</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="15"/>
+        <v>1488587.5999999999</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="15"/>
+        <v>1105478.5999999999</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="15"/>
+        <v>12743301</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="15"/>
+        <v>1501739.1999999997</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="15"/>
+        <v>1579721.1999999997</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="15"/>
+        <v>2116776.8000000003</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="15"/>
+        <v>1783119.8000000003</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="15"/>
+        <v>1763474</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="15"/>
+        <v>2621201.1999999997</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="15"/>
+        <v>3247620.1999999997</v>
+      </c>
+      <c r="R20">
+        <f>ROUNDDOWN(R19+(R22-R17)/5,0)</f>
+        <v>616625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2019</v>
+      </c>
+      <c r="B21">
+        <f>B20+(B22-B17)/5</f>
+        <v>51106515.400000006</v>
+      </c>
+      <c r="C21">
+        <f>C20+(C22-C17)/5</f>
+        <v>9536562.3999999985</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:Q21" si="16">D20+(D22-D17)/5</f>
+        <v>3342458</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="16"/>
+        <v>2399612.4000000004</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="16"/>
+        <v>2898137</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="16"/>
+        <v>1475358.5999999996</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="16"/>
+        <v>1484163.7999999998</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="16"/>
+        <v>1113115.7999999998</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="16"/>
+        <v>13197915</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="16"/>
+        <v>1511814.5999999996</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="16"/>
+        <v>1602242.5999999996</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="16"/>
+        <v>2146368.4000000004</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="16"/>
+        <v>1785086.4000000004</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="16"/>
+        <v>1770799</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="16"/>
+        <v>2628257.5999999996</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="16"/>
+        <v>3276775.5999999996</v>
+      </c>
+      <c r="R21">
+        <f>ROUNDDOWN(R20+(R22-R17)/5,0)</f>
+        <v>644865</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2020</v>
+      </c>
+      <c r="B22" s="1">
+        <v>51738071</v>
+      </c>
+      <c r="C22" s="1">
+        <v>9472127</v>
+      </c>
+      <c r="D22">
+        <v>3324335</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2387911</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2957044</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1475262</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1479740</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1120753</v>
+      </c>
+      <c r="J22" s="1">
+        <v>13652529</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1521890</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1624764</v>
+      </c>
+      <c r="M22" s="1">
+        <v>2175960</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1787053</v>
+      </c>
+      <c r="O22" s="1">
+        <v>1778124</v>
+      </c>
+      <c r="P22" s="1">
+        <v>2635314</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>3305931</v>
+      </c>
+      <c r="R22" s="1">
+        <v>673107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>